<commit_message>
Shemas Elec. Villi-R 28/12/2022 + 8 heures
</commit_message>
<xml_diff>
--- a/villi_R.xlsx
+++ b/villi_R.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\OneDrive\Desktop\VILLI-R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{006AE0B2-134F-4E08-9D41-CDBC2DB02428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F0C60A-386E-46CD-88D3-2B0DE77E9FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1500" windowWidth="20730" windowHeight="11160" xr2:uid="{3D7E3FD7-1512-4C7E-BC22-5D78371FDBF5}"/>
+    <workbookView xWindow="28560" yWindow="1500" windowWidth="20730" windowHeight="11160" xr2:uid="{3D7E3FD7-1512-4C7E-BC22-5D78371FDBF5}"/>
   </bookViews>
   <sheets>
-    <sheet name="CON 12 points" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="CON 15 points" sheetId="1" r:id="rId1"/>
+    <sheet name="inter" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -271,7 +271,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +331,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -548,7 +572,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -563,10 +587,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyBorder="1"/>
@@ -679,6 +701,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1007,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{273EE826-D698-44C0-B80F-988A2F25E318}">
   <dimension ref="B1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,116 +1066,111 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:17" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="19">
         <v>1</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="20">
         <v>2</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="20">
         <v>3</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="20">
         <v>4</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="20">
         <v>5</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="20">
         <v>6</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="20">
         <v>7</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="20">
         <v>8</v>
       </c>
-      <c r="K4" s="22">
+      <c r="K4" s="20">
         <v>9</v>
       </c>
-      <c r="L4" s="22">
+      <c r="L4" s="20">
         <v>10</v>
       </c>
-      <c r="M4" s="22">
+      <c r="M4" s="20">
         <v>11</v>
       </c>
-      <c r="N4" s="22">
+      <c r="N4" s="20">
         <v>12</v>
       </c>
-      <c r="O4" s="22">
+      <c r="O4" s="20">
         <v>13</v>
       </c>
-      <c r="P4" s="22">
+      <c r="P4" s="20">
         <v>14</v>
       </c>
-      <c r="Q4" s="23">
+      <c r="Q4" s="21">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="17"/>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="62">
         <v>0</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="62">
         <v>3100</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="62">
         <v>3101</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="62">
         <v>3104</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="62">
         <v>3105</v>
       </c>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="26"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="24"/>
     </row>
     <row r="9" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:17" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="10"/>
+      <c r="O10" s="60"/>
     </row>
     <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1184,313 +1224,329 @@
       </c>
     </row>
     <row r="13" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="6">
+      <c r="C13" s="58">
         <v>3000</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="59">
         <v>3001</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="59">
         <v>3002</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="59">
         <v>3003</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="59">
         <v>3004</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="59">
         <v>3005</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="8"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="7"/>
     </row>
     <row r="17" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="2:17" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="10"/>
     </row>
     <row r="19" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="51">
         <v>1</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="52">
         <v>2</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="52">
         <v>3</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="52">
         <v>4</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="52">
         <v>5</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="52">
         <v>6</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="52">
         <v>7</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="52">
         <v>8</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="52">
         <v>9</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="52">
         <v>10</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20" s="52">
         <v>11</v>
       </c>
-      <c r="N20" s="4">
+      <c r="N20" s="52">
         <v>12</v>
       </c>
-      <c r="O20" s="4">
+      <c r="O20" s="52">
         <v>13</v>
       </c>
-      <c r="P20" s="4">
+      <c r="P20" s="52">
         <v>14</v>
       </c>
-      <c r="Q20" s="5">
+      <c r="Q20" s="53">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="6">
+      <c r="B21" s="57"/>
+      <c r="C21" s="54">
+        <v>2903</v>
+      </c>
+      <c r="D21" s="55">
+        <v>2904</v>
+      </c>
+      <c r="E21" s="55">
+        <v>2913</v>
+      </c>
+      <c r="F21" s="55">
+        <v>2914</v>
+      </c>
+      <c r="G21" s="55">
+        <v>2932</v>
+      </c>
+      <c r="H21" s="55">
         <v>2990</v>
       </c>
-      <c r="D21" s="7">
+      <c r="I21" s="55">
         <v>2991</v>
       </c>
-      <c r="E21" s="7">
+      <c r="J21" s="55">
         <v>2992</v>
       </c>
-      <c r="F21" s="7">
+      <c r="K21" s="55">
         <v>2993</v>
       </c>
-      <c r="G21" s="7">
+      <c r="L21" s="55">
         <v>2994</v>
       </c>
-      <c r="H21" s="7">
+      <c r="M21" s="55">
         <v>2995</v>
       </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="8"/>
+      <c r="N21" s="55">
+        <v>3023</v>
+      </c>
+      <c r="O21" s="55">
+        <v>3024</v>
+      </c>
+      <c r="P21" s="55">
+        <v>3800</v>
+      </c>
+      <c r="Q21" s="56"/>
     </row>
     <row r="24" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="2:17" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="10"/>
     </row>
     <row r="26" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="19">
         <v>1</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="20">
         <v>2</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="20">
         <v>3</v>
       </c>
-      <c r="F27" s="22">
+      <c r="F27" s="20">
         <v>4</v>
       </c>
-      <c r="G27" s="22">
+      <c r="G27" s="20">
         <v>5</v>
       </c>
-      <c r="H27" s="22">
+      <c r="H27" s="20">
         <v>6</v>
       </c>
-      <c r="I27" s="22">
+      <c r="I27" s="20">
         <v>7</v>
       </c>
-      <c r="J27" s="22">
+      <c r="J27" s="20">
         <v>8</v>
       </c>
-      <c r="K27" s="22">
+      <c r="K27" s="20">
         <v>9</v>
       </c>
-      <c r="L27" s="22">
+      <c r="L27" s="20">
         <v>10</v>
       </c>
-      <c r="M27" s="22">
+      <c r="M27" s="20">
         <v>11</v>
       </c>
-      <c r="N27" s="22">
+      <c r="N27" s="20">
         <v>12</v>
       </c>
-      <c r="O27" s="22">
+      <c r="O27" s="20">
         <v>13</v>
       </c>
-      <c r="P27" s="22">
+      <c r="P27" s="20">
         <v>14</v>
       </c>
-      <c r="Q27" s="23">
+      <c r="Q27" s="21">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="17"/>
-      <c r="C28" s="24" t="s">
+      <c r="B28" s="15"/>
+      <c r="C28" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="23">
         <v>0</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="E28" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="23">
         <v>3104</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="23">
         <v>3105</v>
       </c>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
-      <c r="P28" s="25"/>
-      <c r="Q28" s="26"/>
+      <c r="H28" s="23">
+        <v>3601</v>
+      </c>
+      <c r="I28" s="23">
+        <v>3602</v>
+      </c>
+      <c r="J28" s="23">
+        <v>3603</v>
+      </c>
+      <c r="K28" s="23">
+        <v>3621</v>
+      </c>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="24"/>
     </row>
     <row r="31" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:17" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="10"/>
     </row>
     <row r="33" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="21">
+      <c r="C34" s="19">
         <v>1</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="20">
         <v>2</v>
       </c>
-      <c r="E34" s="22">
+      <c r="E34" s="20">
         <v>3</v>
       </c>
-      <c r="F34" s="22">
+      <c r="F34" s="20">
         <v>4</v>
       </c>
-      <c r="G34" s="22">
+      <c r="G34" s="20">
         <v>5</v>
       </c>
-      <c r="H34" s="22">
+      <c r="H34" s="20">
         <v>6</v>
       </c>
-      <c r="I34" s="22">
+      <c r="I34" s="20">
         <v>7</v>
       </c>
-      <c r="J34" s="22">
+      <c r="J34" s="20">
         <v>8</v>
       </c>
-      <c r="K34" s="22">
+      <c r="K34" s="20">
         <v>9</v>
       </c>
-      <c r="L34" s="22">
+      <c r="L34" s="20">
         <v>10</v>
       </c>
-      <c r="M34" s="22">
+      <c r="M34" s="20">
         <v>11</v>
       </c>
-      <c r="N34" s="22">
+      <c r="N34" s="20">
         <v>12</v>
       </c>
-      <c r="O34" s="22">
+      <c r="O34" s="20">
         <v>13</v>
       </c>
-      <c r="P34" s="22">
+      <c r="P34" s="20">
         <v>14</v>
       </c>
-      <c r="Q34" s="23">
+      <c r="Q34" s="21">
         <v>15</v>
       </c>
     </row>
     <row r="35" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="25" t="s">
+      <c r="D35" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="23">
         <v>0</v>
       </c>
-      <c r="F35" s="25">
+      <c r="F35" s="23">
         <v>3102</v>
       </c>
-      <c r="G35" s="25">
+      <c r="G35" s="23">
         <v>3103</v>
       </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="25"/>
-      <c r="P35" s="25"/>
-      <c r="Q35" s="26"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23"/>
+      <c r="Q35" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1502,8 +1558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5778960-C546-4149-A518-54BC3BE77901}">
   <dimension ref="A3:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,355 +1572,355 @@
   <sheetData>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="40" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="41" t="s">
+      <c r="I4" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="40" t="s">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="O4" s="40" t="s">
+      <c r="O4" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P4" s="16"/>
+      <c r="P4" s="14"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="42"/>
-      <c r="C5" s="36">
+      <c r="B5" s="40"/>
+      <c r="C5" s="34">
         <v>122</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="37" t="s">
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="37" t="s">
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="43"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="41"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
-      <c r="C6" s="36">
+      <c r="B6" s="40"/>
+      <c r="C6" s="34">
         <v>132</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="37" t="s">
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="38" t="s">
+      <c r="L6" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="44" t="s">
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="42" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="37" t="s">
+      <c r="A7" s="25"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37" t="s">
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37" t="s">
+      <c r="I7" s="35"/>
+      <c r="J7" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37" t="s">
+      <c r="L7" s="35"/>
+      <c r="M7" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="37" t="s">
+      <c r="N7" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="O7" s="37" t="s">
+      <c r="O7" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="P7" s="44" t="s">
+      <c r="P7" s="42" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="47" t="s">
+      <c r="C8" s="44"/>
+      <c r="D8" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="E8" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="F8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="47" t="s">
+      <c r="G8" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="47" t="s">
+      <c r="H8" s="17"/>
+      <c r="I8" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="47" t="s">
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="20"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="18"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="28"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="28"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="49" t="s">
+      <c r="F11" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="49" t="s">
+      <c r="G11" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="49" t="s">
+      <c r="H11" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="49" t="s">
+      <c r="I11" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="J11" s="49" t="s">
+      <c r="J11" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="K11" s="49" t="s">
+      <c r="K11" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="L11" s="49" t="s">
+      <c r="L11" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="M11" s="49" t="s">
+      <c r="M11" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="N11" s="49" t="s">
+      <c r="N11" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="O11" s="49" t="s">
+      <c r="O11" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="P11" s="50" t="s">
+      <c r="P11" s="48" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="28"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="28">
+      <c r="B13" s="26"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="26">
         <v>4</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="26">
         <v>4</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="26">
         <v>5</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="26">
         <v>5</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="26">
         <v>6</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I13" s="26">
         <v>7</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="26">
         <v>8</v>
       </c>
-      <c r="K13" s="28">
+      <c r="K13" s="26">
         <v>10</v>
       </c>
-      <c r="L13" s="28">
+      <c r="L13" s="26">
         <v>10</v>
       </c>
-      <c r="M13" s="28">
+      <c r="M13" s="26">
         <v>11</v>
       </c>
-      <c r="N13" s="28">
+      <c r="N13" s="26">
         <v>17</v>
       </c>
-      <c r="O13" s="28">
+      <c r="O13" s="26">
         <v>20</v>
       </c>
-      <c r="P13" s="28">
+      <c r="P13" s="26">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="28"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
-      <c r="C15" s="33" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="30" t="s">
+      <c r="H15" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="30" t="s">
+      <c r="I15" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="K15" s="31" t="s">
+      <c r="K15" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="L15" s="31" t="s">
+      <c r="L15" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="M15" s="31" t="s">
+      <c r="M15" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="N15" s="31" t="s">
+      <c r="N15" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="O15" s="31" t="s">
+      <c r="O15" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="P15" s="32" t="s">
+      <c r="P15" s="30" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>